<commit_message>
fix template, label satuan dan tampilan
</commit_message>
<xml_diff>
--- a/static/assets/file/template.xlsx
+++ b/static/assets/file/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Addh\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Addh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1219B771-7D5B-437E-B49C-FB6DE49AB144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F8F2FF-BF42-4DA1-9097-FD9A85FF30A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{C791BF4A-F1C0-4250-8A4C-F5D9A33581DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C791BF4A-F1C0-4250-8A4C-F5D9A33581DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
   <si>
     <t>mp1</t>
   </si>
@@ -288,13 +288,25 @@
   </si>
   <si>
     <t>gh24</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Catatan</t>
+  </si>
+  <si>
+    <t>Jika nilai adalah data adalah 0 maka beri tanda petik 1 sebelum angka 0</t>
+  </si>
+  <si>
+    <t>If the data value is 0 then put a quotation mark 1 before the number 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +324,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -352,11 +380,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,15 +722,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C822FBD6-BC7F-4685-9B10-29A5CB84F0A8}">
-  <dimension ref="A1:CF2"/>
+  <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:84" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -736,308 +767,359 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+    </row>
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="T7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="U7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="W7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="2" t="s">
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+    </row>
+    <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="R10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="U10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="V10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="W10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="X10" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
-      <c r="AK2" s="3"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="3"/>
-      <c r="AR2" s="3"/>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="3"/>
-      <c r="AU2" s="3"/>
-      <c r="AV2" s="3"/>
-      <c r="AW2" s="3"/>
-      <c r="AX2" s="3"/>
-      <c r="AY2" s="3"/>
-      <c r="AZ2" s="3"/>
-      <c r="BA2" s="3"/>
-      <c r="BB2" s="3"/>
-      <c r="BC2" s="3"/>
-      <c r="BD2" s="3"/>
-      <c r="BE2" s="3"/>
-      <c r="BF2" s="3"/>
-      <c r="BG2" s="3"/>
-      <c r="BH2" s="3"/>
-      <c r="BI2" s="3"/>
-      <c r="BJ2" s="3"/>
-      <c r="BK2" s="3"/>
-      <c r="BL2" s="3"/>
-      <c r="BM2" s="3"/>
-      <c r="BN2" s="3"/>
-      <c r="BO2" s="3"/>
-      <c r="BP2" s="3"/>
-      <c r="BQ2" s="3"/>
-      <c r="BR2" s="3"/>
-      <c r="BS2" s="3"/>
-      <c r="BT2" s="3"/>
-      <c r="BU2" s="3"/>
-      <c r="BV2" s="3"/>
-      <c r="BW2" s="3"/>
-      <c r="BX2" s="3"/>
-      <c r="BY2" s="3"/>
-      <c r="BZ2" s="3"/>
-      <c r="CA2" s="3"/>
-      <c r="CB2" s="3"/>
-      <c r="CC2" s="3"/>
-      <c r="CD2" s="3"/>
-      <c r="CE2" s="3"/>
-      <c r="CF2" s="3"/>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+    </row>
+    <row r="14" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>